<commit_message>
[Include] Sheet with solved questions
</commit_message>
<xml_diff>
--- a/0.bases/Planilha teste calculo e analises - Gabriella Maia.xlsx
+++ b/0.bases/Planilha teste calculo e analises - Gabriella Maia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriellamaia/Documents/desafio_bradesco/0.bases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573CD53D-D32E-0948-B4C4-0FDEE3B4E72B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6634FC-40C5-2F44-82CF-CED71916839A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17080" tabRatio="792" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17080" tabRatio="792" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="O QUE FAZER" sheetId="19" r:id="rId1"/>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="107">
   <si>
     <t>MEDIA RESULTS</t>
   </si>
@@ -407,13 +407,72 @@
   </si>
   <si>
     <t>CPM</t>
+  </si>
+  <si>
+    <t>Investimento Total:</t>
+  </si>
+  <si>
+    <t>Always On</t>
+  </si>
+  <si>
+    <t>Flight Promocional</t>
+  </si>
+  <si>
+    <t>Sites</t>
+  </si>
+  <si>
+    <t>Canais</t>
+  </si>
+  <si>
+    <t>Formatos</t>
+  </si>
+  <si>
+    <t>Coeficiente angular (Clique sobre Investimento)</t>
+  </si>
+  <si>
+    <t>CTR</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CPC Planejado </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Versus</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Realizado</t>
+    </r>
+  </si>
+  <si>
+    <t>CPC Planejado</t>
+  </si>
+  <si>
+    <t>CPC Realizado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="9">
+  <numFmts count="12">
     <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -423,8 +482,11 @@
     <numFmt numFmtId="167" formatCode="&quot;True&quot;;&quot;True&quot;;&quot;False&quot;"/>
     <numFmt numFmtId="168" formatCode="d/m;@"/>
     <numFmt numFmtId="169" formatCode="[$-1010416]#,##0;\-#,##0"/>
+    <numFmt numFmtId="171" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="34" x14ac:knownFonts="1">
+  <fonts count="36" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -636,8 +698,23 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="29">
+  <fills count="31">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -802,6 +879,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -990,7 +1079,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="178">
+  <cellStyleXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1210,8 +1299,9 @@
     <xf numFmtId="43" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1376,21 +1466,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="26" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="26" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="26" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="30" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1409,8 +1484,37 @@
     <xf numFmtId="0" fontId="31" fillId="27" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="149" applyFont="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="34" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="34" fillId="29" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="104" applyFont="1"/>
+    <xf numFmtId="0" fontId="34" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="34" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="149" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="149" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="178" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="178">
+  <cellStyles count="179">
     <cellStyle name="20% - Ênfase1 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="20% - Ênfase1 2 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="20% - Ênfase1 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
@@ -1583,6 +1687,7 @@
     <cellStyle name="srh" xfId="169" xr:uid="{00000000-0005-0000-0000-0000A9000000}"/>
     <cellStyle name="srh 2" xfId="170" xr:uid="{00000000-0005-0000-0000-0000AA000000}"/>
     <cellStyle name="Total" xfId="171" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Vírgula" xfId="178" builtinId="3"/>
     <cellStyle name="Vírgula 2" xfId="172" xr:uid="{00000000-0005-0000-0000-0000AC000000}"/>
     <cellStyle name="Vírgula 2 2" xfId="173" xr:uid="{00000000-0005-0000-0000-0000AD000000}"/>
     <cellStyle name="Vírgula 2 2 2" xfId="174" xr:uid="{00000000-0005-0000-0000-0000AE000000}"/>
@@ -1590,216 +1695,56 @@
     <cellStyle name="Vírgula 3" xfId="176" xr:uid="{00000000-0005-0000-0000-0000B0000000}"/>
     <cellStyle name="Vírgula 4" xfId="177" xr:uid="{00000000-0005-0000-0000-0000B1000000}"/>
   </cellStyles>
-  <dxfs count="70">
+  <dxfs count="5">
     <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="174" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="174" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="174" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="174" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="174" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="174" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="177" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="174" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="177" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="174" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="175" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="174" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="175" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="176" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="174" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="176" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="175" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="174" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="175" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="174" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="174" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="173" formatCode="_-&quot;R$&quot;\ * #,##0.0_-;\-&quot;R$&quot;\ * #,##0.0_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="174" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="173" formatCode="_-&quot;R$&quot;\ * #,##0.0_-;\-&quot;R$&quot;\ * #,##0.0_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode="_-&quot;R$&quot;\ * #,##0.000_-;\-&quot;R$&quot;\ * #,##0.000_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode="_-&quot;R$&quot;\ * #,##0.000_-;\-&quot;R$&quot;\ * #,##0.000_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_-&quot;R$&quot;\ * #,##0.0000_-;\-&quot;R$&quot;\ * #,##0.0000_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode="_-&quot;R$&quot;\ * #,##0.0000_-;\-&quot;R$&quot;\ * #,##0.0000_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode="_-&quot;R$&quot;\ * #,##0.000_-;\-&quot;R$&quot;\ * #,##0.000_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode="_-&quot;R$&quot;\ * #,##0.000_-;\-&quot;R$&quot;\ * #,##0.000_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="#,##0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="#,##0.0"/>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1880,6 +1825,1906 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Always On</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'MEDIA DETAIL RESULTS'!$M$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>investment</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'MEDIA DETAIL RESULTS'!$K$15:$K$19</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4449</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14245</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>120839</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>81348</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36882</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'MEDIA DETAIL RESULTS'!$M$15:$M$19</c:f>
+              <c:numCache>
+                <c:formatCode>"R$"#,##0.00_);[Red]\("R$"#,##0.00\)</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2506.19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12911.58</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40304.862500000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17847.599999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4511</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DBB6-F94C-AA30-D5E0FB22DFFA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1109347792"/>
+        <c:axId val="1041285039"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1109347792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1041285039"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1041285039"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1109347792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Flights Promocional</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'MEDIA DETAIL RESULTS'!$M$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>investment</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'MEDIA DETAIL RESULTS'!$K$27:$K$61</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>54393</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20419</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>179</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4383</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>903</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>558</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>128281</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>587</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65813</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="[$-1010416]#,##0;\-#,##0">
+                  <c:v>3289</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3501</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>412</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'MEDIA DETAIL RESULTS'!$M$27:$M$61</c:f>
+              <c:numCache>
+                <c:formatCode>"R$"#,##0.00_);[Red]\("R$"#,##0.00\)</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>28745.59</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27687.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18814.900000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14211.58</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>508.86</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>277</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1950</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3950</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1960</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>590</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5400</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2405.6480000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>935.21960000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4BBA-EA4A-90B2-87018200C9B4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1025552607"/>
+        <c:axId val="1030607055"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1025552607"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1030607055"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1030607055"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="&quot;R$&quot;#,##0.00_);[Red]\(&quot;R$&quot;#,##0.00\)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1025552607"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2075,10 +3920,103 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
         <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Para melhorar os resultados da Always On a partir dos resultados da Flights Promocional, eu tiraria o formato Search da Always On que parece não estar com bons resultados e usaria a estratégia UOL - Network - Pré roll da Flights Promocional, que tem a melhor CTR, baixo CPC, é de um site que não foi testado na Always On e teve mais que o dobro do esperado na meta de views. </a:t>
+          </a:r>
           <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D5D8004-5BAC-0E4D-B55C-A0C5074067F9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79C99AEF-448E-C14F-9804-0E5DA15349F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2916,8 +4854,8 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2945,25 +4883,40 @@
       <c r="A3" s="56" t="s">
         <v>84</v>
       </c>
+      <c r="B3" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="56" t="s">
         <v>85</v>
       </c>
+      <c r="B4" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="56" t="s">
         <v>88</v>
       </c>
+      <c r="B5" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="56" t="s">
         <v>89</v>
       </c>
+      <c r="B6" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="57" t="s">
         <v>90</v>
+      </c>
+      <c r="B7" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2979,8 +4932,8 @@
   </sheetPr>
   <dimension ref="A1:P63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -3003,21 +4956,21 @@
     <row r="2" spans="1:16" s="4" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="63" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
+      <c r="C2" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
       <c r="P2" s="3"/>
     </row>
     <row r="3" spans="1:16" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3039,10 +4992,10 @@
       <c r="P3" s="3"/>
     </row>
     <row r="4" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="65" t="s">
+      <c r="C4" s="60" t="s">
         <v>91</v>
       </c>
-      <c r="D4" s="66"/>
+      <c r="D4" s="61"/>
       <c r="E4" s="27"/>
       <c r="F4" s="27"/>
       <c r="G4" s="27"/>
@@ -3155,47 +5108,47 @@
       <c r="P11" s="9"/>
     </row>
     <row r="12" spans="1:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C12" s="67" t="s">
+      <c r="C12" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="68"/>
-      <c r="E12" s="68"/>
-      <c r="F12" s="68"/>
-      <c r="G12" s="68"/>
-      <c r="H12" s="68"/>
-      <c r="I12" s="68"/>
-      <c r="J12" s="68"/>
-      <c r="K12" s="68"/>
-      <c r="L12" s="68"/>
-      <c r="M12" s="68"/>
-      <c r="N12" s="68"/>
-      <c r="O12" s="68"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="63"/>
+      <c r="H12" s="63"/>
+      <c r="I12" s="63"/>
+      <c r="J12" s="63"/>
+      <c r="K12" s="63"/>
+      <c r="L12" s="63"/>
+      <c r="M12" s="63"/>
+      <c r="N12" s="63"/>
+      <c r="O12" s="63"/>
       <c r="P12" s="9"/>
     </row>
     <row r="13" spans="1:16" s="11" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="26"/>
       <c r="B13" s="26"/>
-      <c r="C13" s="58" t="s">
+      <c r="C13" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="59"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="58" t="s">
+      <c r="D13" s="65"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="G13" s="59"/>
-      <c r="H13" s="59"/>
-      <c r="I13" s="60"/>
-      <c r="J13" s="58" t="s">
+      <c r="G13" s="65"/>
+      <c r="H13" s="65"/>
+      <c r="I13" s="66"/>
+      <c r="J13" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="K13" s="59"/>
-      <c r="L13" s="60"/>
-      <c r="M13" s="58" t="s">
+      <c r="K13" s="65"/>
+      <c r="L13" s="66"/>
+      <c r="M13" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="N13" s="59"/>
-      <c r="O13" s="59"/>
+      <c r="N13" s="65"/>
+      <c r="O13" s="65"/>
       <c r="P13" s="26"/>
     </row>
     <row r="14" spans="1:16" s="16" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.15">
@@ -3525,44 +5478,44 @@
       <c r="K23"/>
     </row>
     <row r="24" spans="2:16" ht="23" x14ac:dyDescent="0.2">
-      <c r="C24" s="61" t="s">
+      <c r="C24" s="67" t="s">
         <v>80</v>
       </c>
-      <c r="D24" s="62"/>
-      <c r="E24" s="62"/>
-      <c r="F24" s="62"/>
-      <c r="G24" s="62"/>
-      <c r="H24" s="62"/>
-      <c r="I24" s="62"/>
-      <c r="J24" s="62"/>
-      <c r="K24" s="62"/>
-      <c r="L24" s="62"/>
-      <c r="M24" s="62"/>
-      <c r="N24" s="62"/>
-      <c r="O24" s="62"/>
+      <c r="D24" s="68"/>
+      <c r="E24" s="68"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="68"/>
+      <c r="H24" s="68"/>
+      <c r="I24" s="68"/>
+      <c r="J24" s="68"/>
+      <c r="K24" s="68"/>
+      <c r="L24" s="68"/>
+      <c r="M24" s="68"/>
+      <c r="N24" s="68"/>
+      <c r="O24" s="68"/>
     </row>
     <row r="25" spans="2:16" ht="18" x14ac:dyDescent="0.2">
-      <c r="C25" s="58" t="s">
+      <c r="C25" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="59"/>
-      <c r="E25" s="60"/>
-      <c r="F25" s="58" t="s">
+      <c r="D25" s="65"/>
+      <c r="E25" s="66"/>
+      <c r="F25" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="G25" s="59"/>
-      <c r="H25" s="59"/>
-      <c r="I25" s="60"/>
-      <c r="J25" s="58" t="s">
+      <c r="G25" s="65"/>
+      <c r="H25" s="65"/>
+      <c r="I25" s="66"/>
+      <c r="J25" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="K25" s="59"/>
-      <c r="L25" s="60"/>
-      <c r="M25" s="58" t="s">
+      <c r="K25" s="65"/>
+      <c r="L25" s="66"/>
+      <c r="M25" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="N25" s="59"/>
-      <c r="O25" s="59"/>
+      <c r="N25" s="65"/>
+      <c r="O25" s="65"/>
     </row>
     <row r="26" spans="2:16" ht="19" x14ac:dyDescent="0.2">
       <c r="C26" s="45" t="s">
@@ -5236,18 +7189,18 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="12">
+    <mergeCell ref="J25:L25"/>
+    <mergeCell ref="M25:O25"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="C24:O24"/>
     <mergeCell ref="C2:O2"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C12:O12"/>
     <mergeCell ref="J13:L13"/>
     <mergeCell ref="M13:O13"/>
     <mergeCell ref="C13:E13"/>
-    <mergeCell ref="J25:L25"/>
-    <mergeCell ref="M25:O25"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="C24:O24"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="I15:I19">
@@ -5278,14 +7231,1898 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:P68"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B2" s="72" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="73">
+        <f>'MEDIA DETAIL RESULTS'!M20+'MEDIA DETAIL RESULTS'!M62</f>
+        <v>192217.2801</v>
+      </c>
+      <c r="G2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="69">
+        <f>'MEDIA DETAIL RESULTS'!M20</f>
+        <v>78081.232500000013</v>
+      </c>
+      <c r="D3" s="70">
+        <f>C3/$C$2</f>
+        <v>0.40621338757565745</v>
+      </c>
+      <c r="E3" s="70"/>
+      <c r="G3">
+        <f>SLOPE('MEDIA DETAIL RESULTS'!M15:M19,'MEDIA DETAIL RESULTS'!K15:K19)</f>
+        <v>0.27941649859315498</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="69">
+        <f>'MEDIA DETAIL RESULTS'!M62</f>
+        <v>114136.04759999999</v>
+      </c>
+      <c r="D4" s="70">
+        <f>C4/$C$2</f>
+        <v>0.5937866124243425</v>
+      </c>
+      <c r="E4" s="70"/>
+      <c r="G4">
+        <f>SLOPE('MEDIA DETAIL RESULTS'!M27:M61,'MEDIA DETAIL RESULTS'!K27:K61)</f>
+        <v>9.589870662934312E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" s="79" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6"/>
+      <c r="B6" s="77" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="77"/>
+      <c r="D6" s="77"/>
+      <c r="E6" s="77"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="78"/>
+      <c r="H6" s="78"/>
+      <c r="I6" s="78"/>
+      <c r="J6" s="78"/>
+      <c r="K6" s="78"/>
+      <c r="L6" s="78"/>
+      <c r="M6" s="78"/>
+      <c r="N6" s="78"/>
+      <c r="O6" s="78"/>
+      <c r="P6" s="78"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B7" s="75" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" s="75" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="75" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" s="75" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7" s="75"/>
+      <c r="G7" s="75" t="s">
+        <v>99</v>
+      </c>
+      <c r="H7" s="75" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="75" t="s">
+        <v>103</v>
+      </c>
+      <c r="J7" s="75"/>
+      <c r="K7" s="75"/>
+      <c r="L7" s="75" t="s">
+        <v>100</v>
+      </c>
+      <c r="M7" s="75" t="s">
+        <v>5</v>
+      </c>
+      <c r="N7" s="75" t="s">
+        <v>103</v>
+      </c>
+      <c r="O7" s="75"/>
+      <c r="P7" s="75"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!C$15:C$19,'GRAFICOS E ANALISES'!B8,'MEDIA DETAIL RESULTS'!M$15:M$19)</f>
+        <v>2506.19</v>
+      </c>
+      <c r="D8" s="70">
+        <f>C8/$C$12</f>
+        <v>3.2097213629408324E-2</v>
+      </c>
+      <c r="E8" s="80">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!C$15:C$19,'GRAFICOS E ANALISES'!B8,'MEDIA DETAIL RESULTS'!K$15:K$19)/SUMIF('MEDIA DETAIL RESULTS'!C$15:C$19,'GRAFICOS E ANALISES'!B8,'MEDIA DETAIL RESULTS'!J$15:J$19)</f>
+        <v>2.5749120571168624E-3</v>
+      </c>
+      <c r="G8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="76">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!D$15:D$19,'GRAFICOS E ANALISES'!G8,'MEDIA DETAIL RESULTS'!M$15:M$19)</f>
+        <v>15417.77</v>
+      </c>
+      <c r="I8" s="70">
+        <f>H8/H12</f>
+        <v>0.19745807675359123</v>
+      </c>
+      <c r="L8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!E$15:E$19,'GRAFICOS E ANALISES'!L8,'MEDIA DETAIL RESULTS'!M$15:M$19)</f>
+        <v>15417.77</v>
+      </c>
+      <c r="N8" s="70">
+        <f>M8/$M$12</f>
+        <v>0.19745807675359117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!C$15:C$19,'GRAFICOS E ANALISES'!B9,'MEDIA DETAIL RESULTS'!M$15:M$19)</f>
+        <v>12911.58</v>
+      </c>
+      <c r="D9" s="70">
+        <f>C9/$C$12</f>
+        <v>0.16536086312418288</v>
+      </c>
+      <c r="E9" s="80">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!C$15:C$19,'GRAFICOS E ANALISES'!B9,'MEDIA DETAIL RESULTS'!K$15:K$19)/SUMIF('MEDIA DETAIL RESULTS'!C$15:C$19,'GRAFICOS E ANALISES'!B9,'MEDIA DETAIL RESULTS'!J$15:J$19)</f>
+        <v>2.0320912065871423E-2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="76">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!D$15:D$19,'GRAFICOS E ANALISES'!G9,'MEDIA DETAIL RESULTS'!M$15:M$19)</f>
+        <v>62663.462500000001</v>
+      </c>
+      <c r="I9" s="70">
+        <f>H9/H12</f>
+        <v>0.80254192324640883</v>
+      </c>
+      <c r="L9" t="s">
+        <v>24</v>
+      </c>
+      <c r="M9" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!E$15:E$19,'GRAFICOS E ANALISES'!L9,'MEDIA DETAIL RESULTS'!M$15:M$19)</f>
+        <v>40304.862500000003</v>
+      </c>
+      <c r="N9" s="70">
+        <f t="shared" ref="N9:N11" si="0">M9/$M$12</f>
+        <v>0.51619142282365993</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!C$15:C$19,'GRAFICOS E ANALISES'!B10,'MEDIA DETAIL RESULTS'!M$15:M$19)</f>
+        <v>62663.462500000001</v>
+      </c>
+      <c r="D10" s="70">
+        <f>C10/$C$12</f>
+        <v>0.80254192324640883</v>
+      </c>
+      <c r="E10" s="80">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!C$15:C$19,'GRAFICOS E ANALISES'!B10,'MEDIA DETAIL RESULTS'!K$15:K$19)/SUMIF('MEDIA DETAIL RESULTS'!C$15:C$19,'GRAFICOS E ANALISES'!B10,'MEDIA DETAIL RESULTS'!J$15:J$19)</f>
+        <v>4.3247023319915668E-3</v>
+      </c>
+      <c r="L10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M10" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!E$15:E$19,'GRAFICOS E ANALISES'!L10,'MEDIA DETAIL RESULTS'!M$15:M$19)</f>
+        <v>17847.599999999999</v>
+      </c>
+      <c r="N10" s="70">
+        <f t="shared" si="0"/>
+        <v>0.22857733450864773</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="L11" t="s">
+        <v>26</v>
+      </c>
+      <c r="M11" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!E$15:E$19,'GRAFICOS E ANALISES'!L11,'MEDIA DETAIL RESULTS'!M$15:M$19)</f>
+        <v>4511</v>
+      </c>
+      <c r="N11" s="70">
+        <f t="shared" si="0"/>
+        <v>5.7773165914101053E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C12" s="69">
+        <f>SUM(C8:C10)</f>
+        <v>78081.232499999998</v>
+      </c>
+      <c r="H12" s="76">
+        <f>SUM(H8:H9)</f>
+        <v>78081.232499999998</v>
+      </c>
+      <c r="M12" s="74">
+        <f>SUM(M8:M11)</f>
+        <v>78081.232500000013</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" s="79" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14"/>
+      <c r="B14" s="77" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" s="77"/>
+      <c r="D14" s="77"/>
+      <c r="E14" s="77"/>
+      <c r="F14" s="78"/>
+      <c r="G14" s="78"/>
+      <c r="H14" s="78"/>
+      <c r="I14" s="78"/>
+      <c r="J14" s="78"/>
+      <c r="K14" s="78"/>
+      <c r="L14" s="78"/>
+      <c r="M14" s="78"/>
+      <c r="N14" s="78"/>
+      <c r="O14" s="78"/>
+      <c r="P14" s="78"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B15" s="75" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="75" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="75" t="s">
+        <v>103</v>
+      </c>
+      <c r="E15" s="75" t="s">
+        <v>102</v>
+      </c>
+      <c r="F15" s="75"/>
+      <c r="G15" s="75" t="s">
+        <v>99</v>
+      </c>
+      <c r="H15" s="75" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15" s="75" t="s">
+        <v>103</v>
+      </c>
+      <c r="J15" s="75"/>
+      <c r="K15" s="75"/>
+      <c r="L15" s="75" t="s">
+        <v>100</v>
+      </c>
+      <c r="M15" s="75" t="s">
+        <v>5</v>
+      </c>
+      <c r="N15" s="75" t="s">
+        <v>103</v>
+      </c>
+      <c r="O15" s="75"/>
+      <c r="P15" s="75"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B16,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>28745.59</v>
+      </c>
+      <c r="D16" s="70">
+        <f>C16/$C$38</f>
+        <v>0.25185373599707517</v>
+      </c>
+      <c r="E16" s="81">
+        <f>IFERROR(SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B16,'MEDIA DETAIL RESULTS'!K$27:K$61)/SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B16,'MEDIA DETAIL RESULTS'!J$27:J$61),0)</f>
+        <v>2.544816166939716E-3</v>
+      </c>
+      <c r="G16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!D$27:D$61,'GRAFICOS E ANALISES'!G16,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>28745.59</v>
+      </c>
+      <c r="I16" s="70">
+        <f>H16/$H$38</f>
+        <v>0.25185373599707517</v>
+      </c>
+      <c r="L16" t="s">
+        <v>30</v>
+      </c>
+      <c r="M16" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!E$27:E$61,'GRAFICOS E ANALISES'!L16,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>91409.319999999992</v>
+      </c>
+      <c r="N16" s="70">
+        <f>M16/$M$38</f>
+        <v>0.80088036971765619</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B17,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>27687.25</v>
+      </c>
+      <c r="D17" s="70">
+        <f>C17/$C$38</f>
+        <v>0.24258111772918972</v>
+      </c>
+      <c r="E17" s="81">
+        <f>IFERROR(SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B17,'MEDIA DETAIL RESULTS'!K$27:K$61)/SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B17,'MEDIA DETAIL RESULTS'!J$27:J$61),0)</f>
+        <v>1.3325736899741434E-2</v>
+      </c>
+      <c r="G17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!D$27:D$61,'GRAFICOS E ANALISES'!G17,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>27687.25</v>
+      </c>
+      <c r="I17" s="70">
+        <f>H17/$H$38</f>
+        <v>0.24258111772918972</v>
+      </c>
+      <c r="L17" t="s">
+        <v>33</v>
+      </c>
+      <c r="M17" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!E$27:E$61,'GRAFICOS E ANALISES'!L17,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>0</v>
+      </c>
+      <c r="N17" s="70">
+        <f>M17/$M$38</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B18,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="70">
+        <f>C18/$C$38</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="81">
+        <f>IFERROR(SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B18,'MEDIA DETAIL RESULTS'!K$27:K$61)/SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B18,'MEDIA DETAIL RESULTS'!J$27:J$61),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G18" t="s">
+        <v>36</v>
+      </c>
+      <c r="H18" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!D$27:D$61,'GRAFICOS E ANALISES'!G18,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="70">
+        <f>H18/$H$38</f>
+        <v>0</v>
+      </c>
+      <c r="L18" t="s">
+        <v>34</v>
+      </c>
+      <c r="M18" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!E$27:E$61,'GRAFICOS E ANALISES'!L18,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>0</v>
+      </c>
+      <c r="N18" s="70">
+        <f>M18/$M$38</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B19,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="70">
+        <f>C19/$C$38</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="81">
+        <f>IFERROR(SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B19,'MEDIA DETAIL RESULTS'!K$27:K$61)/SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B19,'MEDIA DETAIL RESULTS'!J$27:J$61),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G19" t="s">
+        <v>40</v>
+      </c>
+      <c r="H19" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!D$27:D$61,'GRAFICOS E ANALISES'!G19,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>33535.340000000004</v>
+      </c>
+      <c r="I19" s="70">
+        <f>H19/$H$38</f>
+        <v>0.29381900552161755</v>
+      </c>
+      <c r="L19" t="s">
+        <v>37</v>
+      </c>
+      <c r="M19" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!E$27:E$61,'GRAFICOS E ANALISES'!L19,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>0</v>
+      </c>
+      <c r="N19" s="70">
+        <f>M19/$M$38</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B20,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>33535.340000000004</v>
+      </c>
+      <c r="D20" s="70">
+        <f>C20/$C$38</f>
+        <v>0.29381900552161755</v>
+      </c>
+      <c r="E20" s="81">
+        <f>IFERROR(SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B20,'MEDIA DETAIL RESULTS'!K$27:K$61)/SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B20,'MEDIA DETAIL RESULTS'!J$27:J$61),0)</f>
+        <v>4.9938337988984262E-4</v>
+      </c>
+      <c r="G20" t="s">
+        <v>47</v>
+      </c>
+      <c r="H20" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!D$27:D$61,'GRAFICOS E ANALISES'!G20,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="70">
+        <f>H20/$H$38</f>
+        <v>0</v>
+      </c>
+      <c r="L20" t="s">
+        <v>41</v>
+      </c>
+      <c r="M20" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!E$27:E$61,'GRAFICOS E ANALISES'!L20,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>4549.7276000000002</v>
+      </c>
+      <c r="N20" s="70">
+        <f>M20/$M$38</f>
+        <v>3.9862319535935997E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B21,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>0</v>
+      </c>
+      <c r="D21" s="70">
+        <f>C21/$C$38</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="81">
+        <f>IFERROR(SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B21,'MEDIA DETAIL RESULTS'!K$27:K$61)/SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B21,'MEDIA DETAIL RESULTS'!J$27:J$61),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G21" t="s">
+        <v>48</v>
+      </c>
+      <c r="H21" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!D$27:D$61,'GRAFICOS E ANALISES'!G21,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="70">
+        <f>H21/$H$38</f>
+        <v>0</v>
+      </c>
+      <c r="L21" t="s">
+        <v>43</v>
+      </c>
+      <c r="M21" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!E$27:E$61,'GRAFICOS E ANALISES'!L21,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>0</v>
+      </c>
+      <c r="N21" s="70">
+        <f>M21/$M$38</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B22,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>0</v>
+      </c>
+      <c r="D22" s="70">
+        <f>C22/$C$38</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="81">
+        <f>IFERROR(SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B22,'MEDIA DETAIL RESULTS'!K$27:K$61)/SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B22,'MEDIA DETAIL RESULTS'!J$27:J$61),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G22" t="s">
+        <v>50</v>
+      </c>
+      <c r="H22" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!D$27:D$61,'GRAFICOS E ANALISES'!G22,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="70">
+        <f>H22/$H$38</f>
+        <v>0</v>
+      </c>
+      <c r="L22" t="s">
+        <v>45</v>
+      </c>
+      <c r="M22" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!E$27:E$61,'GRAFICOS E ANALISES'!L22,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>0</v>
+      </c>
+      <c r="N22" s="70">
+        <f>M22/$M$38</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B23,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>0</v>
+      </c>
+      <c r="D23" s="70">
+        <f>C23/$C$38</f>
+        <v>0</v>
+      </c>
+      <c r="E23" s="81">
+        <f>IFERROR(SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B23,'MEDIA DETAIL RESULTS'!K$27:K$61)/SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B23,'MEDIA DETAIL RESULTS'!J$27:J$61),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G23" t="s">
+        <v>58</v>
+      </c>
+      <c r="H23" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!D$27:D$61,'GRAFICOS E ANALISES'!G23,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>0</v>
+      </c>
+      <c r="I23" s="70">
+        <f>H23/$H$38</f>
+        <v>0</v>
+      </c>
+      <c r="L23" t="s">
+        <v>51</v>
+      </c>
+      <c r="M23" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!E$27:E$61,'GRAFICOS E ANALISES'!L23,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>0</v>
+      </c>
+      <c r="N23" s="70">
+        <f>M23/$M$38</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B24,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>0</v>
+      </c>
+      <c r="D24" s="70">
+        <f>C24/$C$38</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="81">
+        <f>IFERROR(SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B24,'MEDIA DETAIL RESULTS'!K$27:K$61)/SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B24,'MEDIA DETAIL RESULTS'!J$27:J$61),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G24" t="s">
+        <v>63</v>
+      </c>
+      <c r="H24" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!D$27:D$61,'GRAFICOS E ANALISES'!G24,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>5827</v>
+      </c>
+      <c r="I24" s="70">
+        <f>H24/$H$38</f>
+        <v>5.105310830826422E-2</v>
+      </c>
+      <c r="L24" t="s">
+        <v>52</v>
+      </c>
+      <c r="M24" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!E$27:E$61,'GRAFICOS E ANALISES'!L24,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>0</v>
+      </c>
+      <c r="N24" s="70">
+        <f>M24/$M$38</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B25,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>0</v>
+      </c>
+      <c r="D25" s="70">
+        <f>C25/$C$38</f>
+        <v>0</v>
+      </c>
+      <c r="E25" s="81">
+        <f>IFERROR(SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B25,'MEDIA DETAIL RESULTS'!K$27:K$61)/SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B25,'MEDIA DETAIL RESULTS'!J$27:J$61),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G25" t="s">
+        <v>65</v>
+      </c>
+      <c r="H25" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!D$27:D$61,'GRAFICOS E ANALISES'!G25,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>1950</v>
+      </c>
+      <c r="I25" s="70">
+        <f>H25/$H$38</f>
+        <v>1.7084874069180578E-2</v>
+      </c>
+      <c r="L25" t="s">
+        <v>54</v>
+      </c>
+      <c r="M25" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!E$27:E$61,'GRAFICOS E ANALISES'!L25,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>277</v>
+      </c>
+      <c r="N25" s="70">
+        <f>M25/$M$38</f>
+        <v>2.4269282652118053E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B26,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>0</v>
+      </c>
+      <c r="D26" s="70">
+        <f>C26/$C$38</f>
+        <v>0</v>
+      </c>
+      <c r="E26" s="81">
+        <f>IFERROR(SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B26,'MEDIA DETAIL RESULTS'!K$27:K$61)/SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B26,'MEDIA DETAIL RESULTS'!J$27:J$61),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G26" t="s">
+        <v>67</v>
+      </c>
+      <c r="H26" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!D$27:D$61,'GRAFICOS E ANALISES'!G26,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>3950</v>
+      </c>
+      <c r="I26" s="70">
+        <f>H26/$H$38</f>
+        <v>3.4607821832442709E-2</v>
+      </c>
+      <c r="L26" t="s">
+        <v>59</v>
+      </c>
+      <c r="M26" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!E$27:E$61,'GRAFICOS E ANALISES'!L26,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>0</v>
+      </c>
+      <c r="N26" s="70">
+        <f>M26/$M$38</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B27,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>0</v>
+      </c>
+      <c r="D27" s="70">
+        <f>C27/$C$38</f>
+        <v>0</v>
+      </c>
+      <c r="E27" s="81">
+        <f>IFERROR(SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B27,'MEDIA DETAIL RESULTS'!K$27:K$61)/SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B27,'MEDIA DETAIL RESULTS'!J$27:J$61),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G27" t="s">
+        <v>75</v>
+      </c>
+      <c r="H27" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!D$27:D$61,'GRAFICOS E ANALISES'!G27,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>9440.8676000000014</v>
+      </c>
+      <c r="I27" s="70">
+        <f>H27/$H$38</f>
+        <v>8.271591489733697E-2</v>
+      </c>
+      <c r="L27" t="s">
+        <v>60</v>
+      </c>
+      <c r="M27" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!E$27:E$61,'GRAFICOS E ANALISES'!L27,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>0</v>
+      </c>
+      <c r="N27" s="70">
+        <f>M27/$M$38</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B28,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="70">
+        <f>C28/$C$38</f>
+        <v>0</v>
+      </c>
+      <c r="E28" s="81">
+        <f>IFERROR(SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B28,'MEDIA DETAIL RESULTS'!K$27:K$61)/SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B28,'MEDIA DETAIL RESULTS'!J$27:J$61),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G28" t="s">
+        <v>77</v>
+      </c>
+      <c r="H28" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!D$27:D$61,'GRAFICOS E ANALISES'!G28,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>3000</v>
+      </c>
+      <c r="I28" s="70">
+        <f>H28/$H$38</f>
+        <v>2.6284421644893197E-2</v>
+      </c>
+      <c r="L28" t="s">
+        <v>62</v>
+      </c>
+      <c r="M28" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!E$27:E$61,'GRAFICOS E ANALISES'!L28,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>0</v>
+      </c>
+      <c r="N28" s="70">
+        <f>M28/$M$38</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B29,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>277</v>
+      </c>
+      <c r="D29" s="70">
+        <f>C29/$C$38</f>
+        <v>2.4269282652118053E-3</v>
+      </c>
+      <c r="E29" s="81">
+        <f>IFERROR(SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B29,'MEDIA DETAIL RESULTS'!K$27:K$61)/SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B29,'MEDIA DETAIL RESULTS'!J$27:J$61),0)</f>
+        <v>6.1145458251239898E-4</v>
+      </c>
+      <c r="I29" s="70"/>
+      <c r="L29" t="s">
+        <v>68</v>
+      </c>
+      <c r="M29" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!E$27:E$61,'GRAFICOS E ANALISES'!L29,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>3950</v>
+      </c>
+      <c r="N29" s="70">
+        <f>M29/$M$38</f>
+        <v>3.4607821832442709E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B30,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>1950</v>
+      </c>
+      <c r="D30" s="70">
+        <f>C30/$C$38</f>
+        <v>1.7084874069180578E-2</v>
+      </c>
+      <c r="E30" s="81">
+        <f>IFERROR(SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B30,'MEDIA DETAIL RESULTS'!K$27:K$61)/SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B30,'MEDIA DETAIL RESULTS'!J$27:J$61),0)</f>
+        <v>5.2241659316239967E-4</v>
+      </c>
+      <c r="L30" t="s">
+        <v>70</v>
+      </c>
+      <c r="M30" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!E$27:E$61,'GRAFICOS E ANALISES'!L30,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>5550</v>
+      </c>
+      <c r="N30" s="70">
+        <f>M30/$M$38</f>
+        <v>4.8626180043052414E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B31,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>3950</v>
+      </c>
+      <c r="D31" s="70">
+        <f>C31/$C$38</f>
+        <v>3.4607821832442709E-2</v>
+      </c>
+      <c r="E31" s="81">
+        <f>IFERROR(SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B31,'MEDIA DETAIL RESULTS'!K$27:K$61)/SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B31,'MEDIA DETAIL RESULTS'!J$27:J$61),0)</f>
+        <v>1.3268611992613805E-4</v>
+      </c>
+      <c r="L31" t="s">
+        <v>76</v>
+      </c>
+      <c r="M31" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!E$27:E$61,'GRAFICOS E ANALISES'!L31,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>5400</v>
+      </c>
+      <c r="N31" s="70">
+        <f>M31/$M$38</f>
+        <v>4.7311958960807754E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B32,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>3000</v>
+      </c>
+      <c r="D32" s="70">
+        <f>C32/$C$38</f>
+        <v>2.6284421644893197E-2</v>
+      </c>
+      <c r="E32" s="81">
+        <f>IFERROR(SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B32,'MEDIA DETAIL RESULTS'!K$27:K$61)/SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B32,'MEDIA DETAIL RESULTS'!J$27:J$61),0)</f>
+        <v>1.5398506172752759E-2</v>
+      </c>
+      <c r="L32" t="s">
+        <v>78</v>
+      </c>
+      <c r="M32" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!E$27:E$61,'GRAFICOS E ANALISES'!L32,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>1000</v>
+      </c>
+      <c r="N32" s="70">
+        <f>M32/$M$38</f>
+        <v>8.7614738816310656E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B33,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>1960</v>
+      </c>
+      <c r="D33" s="70">
+        <f>C33/$C$38</f>
+        <v>1.7172488807996888E-2</v>
+      </c>
+      <c r="E33" s="81">
+        <f>IFERROR(SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B33,'MEDIA DETAIL RESULTS'!K$27:K$61)/SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B33,'MEDIA DETAIL RESULTS'!J$27:J$61),0)</f>
+        <v>1.6779708259778873E-2</v>
+      </c>
+      <c r="L33" t="s">
+        <v>79</v>
+      </c>
+      <c r="M33" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!E$27:E$61,'GRAFICOS E ANALISES'!L33,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>2000</v>
+      </c>
+      <c r="N33" s="70">
+        <f>M33/$M$38</f>
+        <v>1.7522947763262131E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B34,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>590</v>
+      </c>
+      <c r="D34" s="70">
+        <f>C34/$C$38</f>
+        <v>5.1692695901623285E-3</v>
+      </c>
+      <c r="E34" s="81">
+        <f>IFERROR(SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B34,'MEDIA DETAIL RESULTS'!K$27:K$61)/SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B34,'MEDIA DETAIL RESULTS'!J$27:J$61),0)</f>
+        <v>1.5253403313104806E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>82</v>
+      </c>
+      <c r="C35" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B35,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>8100</v>
+      </c>
+      <c r="D35" s="70">
+        <f>C35/$C$38</f>
+        <v>7.0967938441211631E-2</v>
+      </c>
+      <c r="E35" s="81">
+        <f>IFERROR(SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B35,'MEDIA DETAIL RESULTS'!K$27:K$61)/SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B35,'MEDIA DETAIL RESULTS'!J$27:J$61),0)</f>
+        <v>2.294479831617734E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="74">
+        <f>SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B36,'MEDIA DETAIL RESULTS'!M$27:M$61)</f>
+        <v>4340.8675999999996</v>
+      </c>
+      <c r="D36" s="70">
+        <f>C36/$C$38</f>
+        <v>3.8032398101018522E-2</v>
+      </c>
+      <c r="E36" s="81">
+        <f>IFERROR(SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B36,'MEDIA DETAIL RESULTS'!K$27:K$61)/SUMIF('MEDIA DETAIL RESULTS'!C$27:C$61,'GRAFICOS E ANALISES'!B36,'MEDIA DETAIL RESULTS'!J$27:J$61),0)</f>
+        <v>4.1252320986387469E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C38" s="69">
+        <f>SUM(C16:C36)</f>
+        <v>114136.04759999999</v>
+      </c>
+      <c r="H38" s="69">
+        <f>SUM(H16:H28)</f>
+        <v>114136.04759999999</v>
+      </c>
+      <c r="M38" s="74">
+        <f>SUM(M16:M33)</f>
+        <v>114136.04759999999</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B42" s="71" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14" s="71" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="71" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" s="71" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="71" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" s="71" t="s">
+        <v>10</v>
+      </c>
+      <c r="G44" s="71" t="s">
+        <v>11</v>
+      </c>
+      <c r="H44" s="71" t="s">
+        <v>16</v>
+      </c>
+      <c r="I44" s="71" t="s">
+        <v>105</v>
+      </c>
+      <c r="J44" s="71" t="s">
+        <v>106</v>
+      </c>
+      <c r="K44" s="71" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="45" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>17</v>
+      </c>
+      <c r="C45" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" t="s">
+        <v>19</v>
+      </c>
+      <c r="E45" t="s">
+        <v>20</v>
+      </c>
+      <c r="F45" s="82">
+        <v>8333</v>
+      </c>
+      <c r="G45" s="82">
+        <v>4449</v>
+      </c>
+      <c r="H45" s="74">
+        <v>2506.19</v>
+      </c>
+      <c r="I45" s="74">
+        <f>H45/F45</f>
+        <v>0.30075483019320776</v>
+      </c>
+      <c r="J45" s="74">
+        <f>H45/G45</f>
+        <v>0.56331535176444147</v>
+      </c>
+      <c r="K45" s="70">
+        <f>(J45-I45)/I45</f>
+        <v>0.87300516970105635</v>
+      </c>
+    </row>
+    <row r="46" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46" t="s">
+        <v>19</v>
+      </c>
+      <c r="E46" t="s">
+        <v>20</v>
+      </c>
+      <c r="F46" s="82">
+        <v>25000</v>
+      </c>
+      <c r="G46" s="82">
+        <v>14245</v>
+      </c>
+      <c r="H46" s="74">
+        <v>12911.58</v>
+      </c>
+      <c r="I46" s="74">
+        <f t="shared" ref="I46:I49" si="1">H46/F46</f>
+        <v>0.51646320000000001</v>
+      </c>
+      <c r="J46" s="74">
+        <f t="shared" ref="J46:J49" si="2">H46/G46</f>
+        <v>0.90639382239382238</v>
+      </c>
+      <c r="K46" s="70">
+        <f t="shared" ref="K46:K49" si="3">(J46-I46)/I46</f>
+        <v>0.75500175500175493</v>
+      </c>
+    </row>
+    <row r="47" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>81</v>
+      </c>
+      <c r="C47" t="s">
+        <v>23</v>
+      </c>
+      <c r="D47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E47" t="s">
+        <v>20</v>
+      </c>
+      <c r="F47" s="82">
+        <v>117769.57</v>
+      </c>
+      <c r="G47" s="82">
+        <v>120839</v>
+      </c>
+      <c r="H47" s="74">
+        <v>40304.862500000003</v>
+      </c>
+      <c r="I47" s="74">
+        <f t="shared" si="1"/>
+        <v>0.3422349465995333</v>
+      </c>
+      <c r="J47" s="74">
+        <f t="shared" si="2"/>
+        <v>0.33354184079643162</v>
+      </c>
+      <c r="K47" s="70">
+        <f t="shared" si="3"/>
+        <v>-2.5400988091592892E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>81</v>
+      </c>
+      <c r="C48" t="s">
+        <v>23</v>
+      </c>
+      <c r="D48" t="s">
+        <v>25</v>
+      </c>
+      <c r="E48" t="s">
+        <v>20</v>
+      </c>
+      <c r="F48" s="82">
+        <v>40820</v>
+      </c>
+      <c r="G48" s="82">
+        <v>81348</v>
+      </c>
+      <c r="H48" s="74">
+        <v>17847.599999999999</v>
+      </c>
+      <c r="I48" s="74">
+        <f t="shared" si="1"/>
+        <v>0.43722684958353747</v>
+      </c>
+      <c r="J48" s="74">
+        <f t="shared" si="2"/>
+        <v>0.21939814131877855</v>
+      </c>
+      <c r="K48" s="70">
+        <f t="shared" si="3"/>
+        <v>-0.49820524167773028</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>81</v>
+      </c>
+      <c r="C49" t="s">
+        <v>23</v>
+      </c>
+      <c r="D49" t="s">
+        <v>26</v>
+      </c>
+      <c r="E49" t="s">
+        <v>20</v>
+      </c>
+      <c r="F49" s="82">
+        <v>16810.050000000003</v>
+      </c>
+      <c r="G49" s="82">
+        <v>36882</v>
+      </c>
+      <c r="H49" s="74">
+        <v>4511</v>
+      </c>
+      <c r="I49" s="74">
+        <f t="shared" si="1"/>
+        <v>0.26835137313690316</v>
+      </c>
+      <c r="J49" s="74">
+        <f t="shared" si="2"/>
+        <v>0.12230898541293857</v>
+      </c>
+      <c r="K49" s="70">
+        <f t="shared" si="3"/>
+        <v>-0.54422075809337878</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B53" s="71" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" s="71" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="71" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53" s="71" t="s">
+        <v>10</v>
+      </c>
+      <c r="G53" s="71" t="s">
+        <v>11</v>
+      </c>
+      <c r="H53" s="71" t="s">
+        <v>16</v>
+      </c>
+      <c r="I53" s="71" t="s">
+        <v>105</v>
+      </c>
+      <c r="J53" s="71" t="s">
+        <v>106</v>
+      </c>
+      <c r="K53" s="71" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C54" t="s">
+        <v>29</v>
+      </c>
+      <c r="D54" t="s">
+        <v>30</v>
+      </c>
+      <c r="E54" t="s">
+        <v>20</v>
+      </c>
+      <c r="F54" s="82">
+        <v>34261</v>
+      </c>
+      <c r="G54" s="82">
+        <v>54393</v>
+      </c>
+      <c r="H54" s="74">
+        <v>28745.59</v>
+      </c>
+      <c r="I54" s="74">
+        <f>H54/F54</f>
+        <v>0.8390178336884504</v>
+      </c>
+      <c r="J54" s="74">
+        <f>H54/G54</f>
+        <v>0.5284795837699704</v>
+      </c>
+      <c r="K54" s="70">
+        <f>(J54-I54)/I54</f>
+        <v>-0.37012115529571821</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>31</v>
+      </c>
+      <c r="C55" t="s">
+        <v>23</v>
+      </c>
+      <c r="D55" t="s">
+        <v>30</v>
+      </c>
+      <c r="E55" t="s">
+        <v>32</v>
+      </c>
+      <c r="F55" s="82">
+        <v>124380</v>
+      </c>
+      <c r="G55" s="82">
+        <v>135760</v>
+      </c>
+      <c r="H55" s="74">
+        <v>27687.25</v>
+      </c>
+      <c r="I55" s="74">
+        <f t="shared" ref="I55:I68" si="4">H55/F55</f>
+        <v>0.22260210644798198</v>
+      </c>
+      <c r="J55" s="74">
+        <f t="shared" ref="J55:J68" si="5">H55/G55</f>
+        <v>0.20394261932822627</v>
+      </c>
+      <c r="K55" s="70">
+        <f t="shared" ref="K55:K68" si="6">(J55-I55)/I55</f>
+        <v>-8.3824395992928694E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>39</v>
+      </c>
+      <c r="C56" t="s">
+        <v>40</v>
+      </c>
+      <c r="D56" t="s">
+        <v>30</v>
+      </c>
+      <c r="E56" t="s">
+        <v>38</v>
+      </c>
+      <c r="F56" s="82">
+        <v>820313</v>
+      </c>
+      <c r="G56" s="82">
+        <v>1235539</v>
+      </c>
+      <c r="H56" s="74">
+        <v>18814.900000000001</v>
+      </c>
+      <c r="I56" s="74">
+        <f t="shared" si="4"/>
+        <v>2.2936245067431579E-2</v>
+      </c>
+      <c r="J56" s="74">
+        <f t="shared" si="5"/>
+        <v>1.5228090736107886E-2</v>
+      </c>
+      <c r="K56" s="70">
+        <f t="shared" si="6"/>
+        <v>-0.33606871171205438</v>
+      </c>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>39</v>
+      </c>
+      <c r="C57" t="s">
+        <v>40</v>
+      </c>
+      <c r="D57" t="s">
+        <v>30</v>
+      </c>
+      <c r="E57" t="s">
+        <v>38</v>
+      </c>
+      <c r="F57" s="82">
+        <v>820313</v>
+      </c>
+      <c r="G57" s="82">
+        <v>1188405</v>
+      </c>
+      <c r="H57" s="74">
+        <v>14211.58</v>
+      </c>
+      <c r="I57" s="74">
+        <f t="shared" si="4"/>
+        <v>1.7324582202159419E-2</v>
+      </c>
+      <c r="J57" s="74">
+        <f t="shared" si="5"/>
+        <v>1.1958532655113365E-2</v>
+      </c>
+      <c r="K57" s="70">
+        <f t="shared" si="6"/>
+        <v>-0.30973615896937495</v>
+      </c>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
+        <v>39</v>
+      </c>
+      <c r="C58" t="s">
+        <v>40</v>
+      </c>
+      <c r="D58" t="s">
+        <v>41</v>
+      </c>
+      <c r="E58" t="s">
+        <v>38</v>
+      </c>
+      <c r="F58" s="82">
+        <v>1136358</v>
+      </c>
+      <c r="G58" s="82">
+        <v>237338</v>
+      </c>
+      <c r="H58" s="74">
+        <v>508.86</v>
+      </c>
+      <c r="I58" s="74">
+        <f t="shared" si="4"/>
+        <v>4.4779902108314459E-4</v>
+      </c>
+      <c r="J58" s="74">
+        <f t="shared" si="5"/>
+        <v>2.1440308757973859E-3</v>
+      </c>
+      <c r="K58" s="70">
+        <f t="shared" si="6"/>
+        <v>3.7879311361855241</v>
+      </c>
+    </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
+        <v>86</v>
+      </c>
+      <c r="C59" t="s">
+        <v>63</v>
+      </c>
+      <c r="D59" t="s">
+        <v>54</v>
+      </c>
+      <c r="E59" t="s">
+        <v>38</v>
+      </c>
+      <c r="F59" s="82">
+        <v>15000</v>
+      </c>
+      <c r="G59" s="82">
+        <v>14719</v>
+      </c>
+      <c r="H59" s="74">
+        <v>277</v>
+      </c>
+      <c r="I59" s="74">
+        <f t="shared" si="4"/>
+        <v>1.8466666666666666E-2</v>
+      </c>
+      <c r="J59" s="74">
+        <f t="shared" si="5"/>
+        <v>1.8819213261770502E-2</v>
+      </c>
+      <c r="K59" s="70">
+        <f t="shared" si="6"/>
+        <v>1.9090970853998364E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
+        <v>64</v>
+      </c>
+      <c r="C60" t="s">
+        <v>65</v>
+      </c>
+      <c r="D60" t="s">
+        <v>30</v>
+      </c>
+      <c r="E60" t="s">
+        <v>38</v>
+      </c>
+      <c r="F60" s="82">
+        <v>250000</v>
+      </c>
+      <c r="G60" s="82">
+        <v>264157</v>
+      </c>
+      <c r="H60" s="74">
+        <v>1950</v>
+      </c>
+      <c r="I60" s="74">
+        <f t="shared" si="4"/>
+        <v>7.7999999999999996E-3</v>
+      </c>
+      <c r="J60" s="74">
+        <f t="shared" si="5"/>
+        <v>7.3819735990339076E-3</v>
+      </c>
+      <c r="K60" s="70">
+        <f t="shared" si="6"/>
+        <v>-5.3593128328986168E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
+        <v>66</v>
+      </c>
+      <c r="C61" t="s">
+        <v>67</v>
+      </c>
+      <c r="D61" t="s">
+        <v>68</v>
+      </c>
+      <c r="E61" t="s">
+        <v>38</v>
+      </c>
+      <c r="F61" s="82">
+        <v>250000</v>
+      </c>
+      <c r="G61" s="82">
+        <v>271317</v>
+      </c>
+      <c r="H61" s="74">
+        <v>3950</v>
+      </c>
+      <c r="I61" s="74">
+        <f t="shared" si="4"/>
+        <v>1.5800000000000002E-2</v>
+      </c>
+      <c r="J61" s="74">
+        <f t="shared" si="5"/>
+        <v>1.4558615936340148E-2</v>
+      </c>
+      <c r="K61" s="70">
+        <f t="shared" si="6"/>
+        <v>-7.8568611624041343E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B62" t="s">
+        <v>82</v>
+      </c>
+      <c r="C62" t="s">
+        <v>75</v>
+      </c>
+      <c r="D62" t="s">
+        <v>76</v>
+      </c>
+      <c r="E62" t="s">
+        <v>32</v>
+      </c>
+      <c r="F62" s="82">
+        <v>981250</v>
+      </c>
+      <c r="G62" s="82">
+        <v>2672571</v>
+      </c>
+      <c r="H62" s="74">
+        <v>5400</v>
+      </c>
+      <c r="I62" s="74">
+        <f t="shared" si="4"/>
+        <v>5.5031847133757963E-3</v>
+      </c>
+      <c r="J62" s="74">
+        <f t="shared" si="5"/>
+        <v>2.020526302201139E-3</v>
+      </c>
+      <c r="K62" s="70">
+        <f t="shared" si="6"/>
+        <v>-0.63284417888243194</v>
+      </c>
+    </row>
+    <row r="63" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B63" t="s">
+        <v>82</v>
+      </c>
+      <c r="C63" t="s">
+        <v>75</v>
+      </c>
+      <c r="D63" t="s">
+        <v>41</v>
+      </c>
+      <c r="E63" t="s">
+        <v>38</v>
+      </c>
+      <c r="F63" s="82">
+        <v>981250</v>
+      </c>
+      <c r="G63" s="82">
+        <v>2903568</v>
+      </c>
+      <c r="H63" s="74">
+        <v>700</v>
+      </c>
+      <c r="I63" s="74">
+        <f t="shared" si="4"/>
+        <v>7.1337579617834399E-4</v>
+      </c>
+      <c r="J63" s="74">
+        <f t="shared" si="5"/>
+        <v>2.4108269549740182E-4</v>
+      </c>
+      <c r="K63" s="70">
+        <f t="shared" si="6"/>
+        <v>-0.66205372149024921</v>
+      </c>
+    </row>
+    <row r="64" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B64" t="s">
+        <v>74</v>
+      </c>
+      <c r="C64" t="s">
+        <v>75</v>
+      </c>
+      <c r="D64" t="s">
+        <v>41</v>
+      </c>
+      <c r="E64" t="s">
+        <v>38</v>
+      </c>
+      <c r="F64" s="82">
+        <v>2292137</v>
+      </c>
+      <c r="G64" s="82">
+        <v>9127452</v>
+      </c>
+      <c r="H64" s="74">
+        <v>2405.6480000000001</v>
+      </c>
+      <c r="I64" s="74">
+        <f t="shared" si="4"/>
+        <v>1.0495219090307429E-3</v>
+      </c>
+      <c r="J64" s="74">
+        <f t="shared" si="5"/>
+        <v>2.6356183521973056E-4</v>
+      </c>
+      <c r="K64" s="70">
+        <f t="shared" si="6"/>
+        <v>-0.74887438465850054</v>
+      </c>
+    </row>
+    <row r="65" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B65" t="s">
+        <v>74</v>
+      </c>
+      <c r="C65" t="s">
+        <v>75</v>
+      </c>
+      <c r="D65" t="s">
+        <v>41</v>
+      </c>
+      <c r="E65" t="s">
+        <v>38</v>
+      </c>
+      <c r="F65" s="82">
+        <v>2292138</v>
+      </c>
+      <c r="G65" s="82">
+        <v>8173933</v>
+      </c>
+      <c r="H65" s="74">
+        <v>935.21960000000001</v>
+      </c>
+      <c r="I65" s="74">
+        <f t="shared" si="4"/>
+        <v>4.0801190853255784E-4</v>
+      </c>
+      <c r="J65" s="74">
+        <f t="shared" si="5"/>
+        <v>1.1441488448706395E-4</v>
+      </c>
+      <c r="K65" s="70">
+        <f t="shared" si="6"/>
+        <v>-0.719579546345682</v>
+      </c>
+    </row>
+    <row r="66" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B66" t="s">
+        <v>74</v>
+      </c>
+      <c r="C66" t="s">
+        <v>77</v>
+      </c>
+      <c r="D66" t="s">
+        <v>78</v>
+      </c>
+      <c r="E66" t="s">
+        <v>32</v>
+      </c>
+      <c r="F66" s="82">
+        <v>226041</v>
+      </c>
+      <c r="G66" s="82">
+        <v>298352</v>
+      </c>
+      <c r="H66" s="74">
+        <v>1000</v>
+      </c>
+      <c r="I66" s="74">
+        <f t="shared" si="4"/>
+        <v>4.42397618131224E-3</v>
+      </c>
+      <c r="J66" s="74">
+        <f t="shared" si="5"/>
+        <v>3.3517455891028049E-3</v>
+      </c>
+      <c r="K66" s="70">
+        <f t="shared" si="6"/>
+        <v>-0.2423680752936129</v>
+      </c>
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B67" t="s">
+        <v>82</v>
+      </c>
+      <c r="C67" t="s">
+        <v>77</v>
+      </c>
+      <c r="D67" t="s">
+        <v>79</v>
+      </c>
+      <c r="E67" t="s">
+        <v>38</v>
+      </c>
+      <c r="F67" s="82">
+        <v>142248</v>
+      </c>
+      <c r="G67" s="82">
+        <v>58483</v>
+      </c>
+      <c r="H67" s="74">
+        <v>1000</v>
+      </c>
+      <c r="I67" s="74">
+        <f t="shared" si="4"/>
+        <v>7.0299758168831895E-3</v>
+      </c>
+      <c r="J67" s="74">
+        <f t="shared" si="5"/>
+        <v>1.7098986030128414E-2</v>
+      </c>
+      <c r="K67" s="70">
+        <f t="shared" si="6"/>
+        <v>1.4322965648137067</v>
+      </c>
+    </row>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B68" t="s">
+        <v>82</v>
+      </c>
+      <c r="C68" t="s">
+        <v>77</v>
+      </c>
+      <c r="D68" t="s">
+        <v>79</v>
+      </c>
+      <c r="E68" t="s">
+        <v>38</v>
+      </c>
+      <c r="F68" s="82">
+        <v>142248</v>
+      </c>
+      <c r="G68" s="82">
+        <v>1601</v>
+      </c>
+      <c r="H68" s="74">
+        <v>1000</v>
+      </c>
+      <c r="I68" s="74">
+        <f t="shared" si="4"/>
+        <v>7.0299758168831895E-3</v>
+      </c>
+      <c r="J68" s="74">
+        <f t="shared" si="5"/>
+        <v>0.62460961898813239</v>
+      </c>
+      <c r="K68" s="70">
+        <f t="shared" si="6"/>
+        <v>87.849469081823869</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D3:E4">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8:D10">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16:D36">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I8:I9">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16:I28">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N8:N11">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N16:N33">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K54:K68">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K45:K49">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>